<commit_message>
Sync data dictionaries from public_api_docs
</commit_message>
<xml_diff>
--- a/data_dictionaries/en/Belvo_Data_Dictionary_en.xlsx
+++ b/data_dictionaries/en/Belvo_Data_Dictionary_en.xlsx
@@ -27089,7 +27089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27499,7 +27499,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>48572</t>
+          <t>48572.01</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -27538,7 +27538,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>21345</t>
+          <t>21345.01</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -27577,7 +27577,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>154321</t>
+          <t>154321.01</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -27616,7 +27616,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>31789</t>
+          <t>31789.01</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -27655,7 +27655,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>12345.01</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
@@ -27694,7 +27694,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
@@ -27733,7 +27733,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>8976</t>
+          <t>8976.01</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>65432</t>
+          <t>65432.01</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -27811,7 +27811,7 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>14321</t>
+          <t>14321.01</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
@@ -27850,7 +27850,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>54321</t>
+          <t>54321.01</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -27889,7 +27889,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>372480</t>
+          <t>372480.01</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -27959,7 +27959,7 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>1123456</t>
+          <t>1123456.01</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
@@ -27988,17 +27988,17 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.long_term_accounts_receivable</t>
+          <t>balance_sheet.non_current_assets.accumulated_depreciation_and_amortization</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>The amount owed by customers for sales made on credit, expected to be received after one year.</t>
+          <t>Total accumulated depreciation and amortization, representing the cumulative allocation of the cost of non-current assets over the period they are expected to provide economic benefits.</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>10987</t>
+          <t>123456.01</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
@@ -28027,17 +28027,17 @@
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.prepayment_to_suppliers</t>
+          <t>balance_sheet.non_current_assets.long_term_accounts_receivable</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>The amount paid in advance to suppliers for goods or services to be received in the future, expected to be utilized over the long term.</t>
+          <t>The amount owed by customers for sales made on credit, expected to be received after one year.</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>5432</t>
+          <t>10987.01</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
@@ -28066,17 +28066,17 @@
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.goodwill</t>
+          <t>balance_sheet.non_current_assets.prepayment_to_suppliers</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>The value of intangible assets that arise from the acquisition of other companies, representing the premium paid over the fair value of net assets acquired.</t>
+          <t>The amount paid in advance to suppliers for goods or services to be received in the future, expected to be utilized over the long term.</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>47654</t>
+          <t>5432.01</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
@@ -28105,17 +28105,17 @@
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.intangible_assets</t>
+          <t>balance_sheet.non_current_assets.goodwill</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>The total value of intangible assets owned by the company, such as patents, trademarks, and copyrights, with useful lives extending beyond one year.</t>
+          <t>The value of intangible assets that arise from the acquisition of other companies, representing the premium paid over the fair value of net assets acquired.</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>43210</t>
+          <t>47654.01</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
@@ -28144,17 +28144,17 @@
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.investments_in_associates</t>
+          <t>balance_sheet.non_current_assets.intangible_assets</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>The value of investments in other companies in which the company has significant influence but not control, typically represented by ownership of 20-50% of the associate's voting shares.</t>
+          <t>The total value of intangible assets owned by the company, such as patents, trademarks, and copyrights, with useful lives extending beyond one year.</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>65432</t>
+          <t>43210.01</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
@@ -28183,17 +28183,17 @@
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.long_term_financial_instruments</t>
+          <t>balance_sheet.non_current_assets.investments_in_associates</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>The value of financial instruments that are expected to be held for more than one year, such as bonds, debentures, and long-term loans.</t>
+          <t>The value of investments in other companies in which the company has significant influence but not control, typically represented by ownership of 20-50% of the associate's voting shares.</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>32876</t>
+          <t>65432.01</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
@@ -28222,17 +28222,17 @@
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_assets.total</t>
+          <t>balance_sheet.non_current_assets.long_term_financial_instruments</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>The sum of all non-current assets, representing the total value of assets expected to be used or held for more than one year.</t>
+          <t>The value of financial instruments that are expected to be held for more than one year, such as bonds, debentures, and long-term loans.</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>1346647</t>
+          <t>32876.01</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
@@ -28261,29 +28261,37 @@
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities</t>
+          <t>balance_sheet.non_current_assets.total</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>The current liabilities of the company, expected to be settled within the given year.</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr"/>
+          <t>The sum of all non-current assets, representing the total value of assets expected to be used or held for more than one year.</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>1346647.01</t>
+        </is>
+      </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="inlineStr"/>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H31" s="2" t="inlineStr"/>
@@ -28292,37 +28300,29 @@
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.bank_loans</t>
+          <t>balance_sheet.current_liabilities</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>The total amount of loans borrowed from banks or financial institutions, expected to be repaid within one year.</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>49876</t>
-        </is>
-      </c>
+          <t>The current liabilities of the company, expected to be settled within the given year.</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr"/>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr"/>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H32" s="2" t="inlineStr"/>
@@ -28331,17 +28331,17 @@
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.accounts_payable</t>
+          <t>balance_sheet.current_liabilities.bank_loans</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>The amount owed to suppliers for goods or services purchased on credit, expected to be paid within a short period.</t>
+          <t>The total amount of loans borrowed from banks or financial institutions, expected to be repaid within one year.</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>103298</t>
+          <t>49876.01</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
@@ -28370,17 +28370,17 @@
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.notes_payable</t>
+          <t>balance_sheet.current_liabilities.accounts_payable</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>The value of written promissory notes issued to suppliers or others, promising to pay a specified amount by a certain date.</t>
+          <t>The amount owed to suppliers for goods or services purchased on credit, expected to be paid within a short period.</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>25643</t>
+          <t>103298.01</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
@@ -28409,17 +28409,17 @@
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.financial_instruments</t>
+          <t>balance_sheet.current_liabilities.notes_payable</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>The value of financial instruments that are expected to be liquidated into cash within one year, such as bonds, debentures, and short-term loans.</t>
+          <t>The value of written promissory notes issued to suppliers or others, promising to pay a specified amount by a certain date.</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>14321</t>
+          <t>25643.01</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
@@ -28448,17 +28448,17 @@
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.other_creditors</t>
+          <t>balance_sheet.current_liabilities.financial_instruments</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>The total amounts due to various other creditors, excluding accounts and notes payable.</t>
+          <t>The value of financial instruments that are expected to be liquidated into cash within one year, such as bonds, debentures, and short-term loans.</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>21987</t>
+          <t>14321.01</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
@@ -28487,17 +28487,17 @@
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.income_tax_payable</t>
+          <t>balance_sheet.current_liabilities.other_creditors</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>The amount of income tax that is owed to tax authorities, expected to be paid within a short period.</t>
+          <t>The total amounts due to various other creditors, excluding accounts and notes payable.</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>12765</t>
+          <t>21987.01</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
@@ -28526,17 +28526,17 @@
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.customer_advances</t>
+          <t>balance_sheet.current_liabilities.income_tax_payable</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>The total amount received in advance from customers for goods or services to be delivered in the future, expected to be utilized within one year.</t>
+          <t>The amount of income tax that is owed to tax authorities, expected to be paid within a short period.</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>18765</t>
+          <t>12765.01</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
@@ -28565,17 +28565,17 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.provisions</t>
+          <t>balance_sheet.current_liabilities.customer_advances</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>The estimated amount set aside for future liabilities or losses, such as warranties, legal claims, or restructuring costs.</t>
+          <t>The total amount received in advance from customers for goods or services to be delivered in the future, expected to be utilized within one year.</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>10987</t>
+          <t>18765.01</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -28604,17 +28604,17 @@
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.taxes_payable</t>
+          <t>balance_sheet.current_liabilities.provisions</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>The total amount of taxes owed to tax authorities, expected to be paid within a short period.</t>
+          <t>The estimated amount set aside for future liabilities or losses, such as warranties, legal claims, or restructuring costs.</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>5321</t>
+          <t>10987.01</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -28643,17 +28643,17 @@
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.current_liabilities.total</t>
+          <t>balance_sheet.current_liabilities.taxes_payable</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>The sum of all current liabilities, representing the total value of obligations expected to be settled within one year.</t>
+          <t>The total amount of taxes owed to tax authorities, expected to be paid within a short period.</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>260963</t>
+          <t>5321.01</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
@@ -28682,29 +28682,37 @@
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities</t>
+          <t>balance_sheet.current_liabilities.total</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>The non-current liabilities of the company, which are long-term obligations not due within the given year.</t>
-        </is>
-      </c>
-      <c r="C42" s="2" t="inlineStr"/>
+          <t>The sum of all current liabilities, representing the total value of obligations expected to be settled within one year.</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>260963.01</t>
+        </is>
+      </c>
       <c r="D42" s="2" t="inlineStr">
         <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="E42" s="2" t="inlineStr"/>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H42" s="2" t="inlineStr"/>
@@ -28713,37 +28721,29 @@
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.long_term_accounts_payable</t>
+          <t>balance_sheet.non_current_liabilities</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>The amount owed to suppliers for goods or services purchased on credit, expected to be paid after one year.</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>30876</t>
-        </is>
-      </c>
+          <t>The non-current liabilities of the company, which are long-term obligations not due within the given year.</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="inlineStr"/>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E43" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr"/>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H43" s="2" t="inlineStr"/>
@@ -28752,17 +28752,17 @@
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.long_term_financial_instruments</t>
+          <t>balance_sheet.non_current_liabilities.long_term_accounts_payable</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>The value of financial instruments that are expected to be held for more than one year, such as bonds, debentures, and long-term loans.</t>
+          <t>The amount owed to suppliers for goods or services purchased on credit, expected to be paid after one year.</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>42310</t>
+          <t>30876.01</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr">
@@ -28791,17 +28791,17 @@
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.deferred_revenue</t>
+          <t>balance_sheet.non_current_liabilities.long_term_financial_instruments</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>The amount received in advance from customers for goods or services to be delivered in the future, expected to be recognized as revenue over the long term (such as rent).</t>
+          <t>The value of financial instruments that are expected to be held for more than one year, such as bonds, debentures, and long-term loans.</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>21987</t>
+          <t>42310.01</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
@@ -28830,17 +28830,17 @@
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.contributions_for_future_capital_increases</t>
+          <t>balance_sheet.non_current_liabilities.deferred_revenue</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>The total contributions received from shareholders or other investors for future capital increases, expected to be utilized over the long term.</t>
+          <t>The amount received in advance from customers for goods or services to be delivered in the future, expected to be recognized as revenue over the long term (such as rent).</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>10987</t>
+          <t>21987.01</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
@@ -28869,17 +28869,17 @@
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.deferred_income_tax</t>
+          <t>balance_sheet.non_current_liabilities.contributions_for_future_capital_increases</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>The amount of income tax that is deferred to future periods, expected to be paid after one year.</t>
+          <t>The total contributions received from shareholders or other investors for future capital increases, expected to be utilized over the long term.</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>26543</t>
+          <t>10987.01</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
@@ -28908,17 +28908,17 @@
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.employee_benefits</t>
+          <t>balance_sheet.non_current_liabilities.deferred_income_tax</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>The total amount of benefits owed to employees, such as pensions, gratuities, and other post-employment benefits, expected to be settled over the long term.</t>
+          <t>The amount of income tax that is deferred to future periods, expected to be paid after one year.</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>30218</t>
+          <t>26543.01</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
@@ -28947,17 +28947,17 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.long_term_provisions</t>
+          <t>balance_sheet.non_current_liabilities.employee_benefits</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>The estimated amount set aside for future liabilities or losses, such as warranties, legal claims, or restructuring costs, expected to be settled after one year.</t>
+          <t>The total amount of benefits owed to employees, such as pensions, gratuities, and other post-employment benefits, expected to be settled over the long term.</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>15432</t>
+          <t>30218.01</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
@@ -28986,17 +28986,17 @@
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.non_current_liabilities.total</t>
+          <t>balance_sheet.non_current_liabilities.long_term_provisions</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>The sum of all non-current liabilities, representing the total value of obligations expected to be settled after one year.</t>
+          <t>The estimated amount set aside for future liabilities or losses, such as warranties, legal claims, or restructuring costs, expected to be settled after one year.</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>178353</t>
+          <t>15432.01</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr">
@@ -29025,29 +29025,37 @@
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity</t>
+          <t>balance_sheet.non_current_liabilities.total</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>The equity of the company, representing the residual interest in the assets after deducting liabilities.</t>
-        </is>
-      </c>
-      <c r="C51" s="2" t="inlineStr"/>
+          <t>The sum of all non-current liabilities, representing the total value of obligations expected to be settled after one year.</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="inlineStr">
+        <is>
+          <t>178353.01</t>
+        </is>
+      </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="E51" s="2" t="inlineStr"/>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H51" s="2" t="inlineStr"/>
@@ -29056,37 +29064,29 @@
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity.stockholders_equity</t>
+          <t>balance_sheet.equity</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>The total value of shares issued by the company, representing the ownership interest of shareholders in the business.</t>
-        </is>
-      </c>
-      <c r="C52" s="2" t="inlineStr">
-        <is>
-          <t>501234</t>
-        </is>
-      </c>
+          <t>The equity of the company, representing the residual interest in the assets after deducting liabilities.</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr"/>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E52" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr"/>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H52" s="2" t="inlineStr"/>
@@ -29095,17 +29095,17 @@
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity.retained_earnings</t>
+          <t>balance_sheet.equity.stockholders_equity</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>The accumulated profits or losses of the company that have not been distributed to shareholders as dividends.</t>
+          <t>The total value of shares issued by the company, representing the ownership interest of shareholders in the business.</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>202345</t>
+          <t>501234.01</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
@@ -29134,17 +29134,17 @@
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity.other_comprehensive_income</t>
+          <t>balance_sheet.equity.future_capital_contributions</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>The gains or losses that are not included in net income but are reported directly in equity, such as unrealized gains on investments or foreign currency translation adjustments.</t>
+          <t>The funds received from shareholders that are specifically designated for future capital increases or investments.</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>10987</t>
+          <t>75000.01</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
@@ -29173,17 +29173,17 @@
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity.controlling_interest</t>
+          <t>balance_sheet.equity.legal_reserve</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>The ownership interest in the company held by the parent entity or majority shareholders, representing the controlling stake in the business.</t>
+          <t>The statutory reserve mandated by law, typically set aside from profits, to provide financial protection against future losses or obligations.</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>70876</t>
+          <t>25000.01</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
@@ -29212,17 +29212,17 @@
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity.non_controlling_interest</t>
+          <t>balance_sheet.equity.capital_update_excess</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>The ownership interest in the company held by minority shareholders, representing the non-controlling stake in the business.</t>
+          <t>The surplus resulting from adjustments made to equity capital, often due to inflation or the revaluation of assets.</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>50321</t>
+          <t>15000.01</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
@@ -29251,17 +29251,17 @@
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>balance_sheet.equity.total</t>
+          <t>balance_sheet.equity.capital_update_insufficiency</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>The sum of share capital, retained earnings, other comprehensive income, controlling interest, and non-controlling interest, representing the total equity of the company.</t>
+          <t>The deficit resulting from adjustments made to equity capital, often due to inflation or the revaluation of assets.</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>836763</t>
+          <t>-5000.01</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
@@ -29290,21 +29290,29 @@
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>income_statement</t>
+          <t>balance_sheet.equity.capital_reserve</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>The income statement detailing the company's revenues, expenses, and profits for the given year.</t>
-        </is>
-      </c>
-      <c r="C58" s="2" t="inlineStr"/>
+          <t>The equity reserve derived from non-operating activities, such as gains from asset revaluations or certain capital transactions.</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>10000.01</t>
+        </is>
+      </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="E58" s="2" t="inlineStr"/>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -29312,7 +29320,7 @@
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H58" s="2" t="inlineStr"/>
@@ -29321,290 +29329,286 @@
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
+          <t>balance_sheet.equity.share_premium_on_stock_sales</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>The excess amount received by a company when shares are issued at a price above their nominal (par) value.</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>50000.01</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G59" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H59" s="2" t="inlineStr"/>
+      <c r="I59" s="2" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>balance_sheet.equity.retained_earnings</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>The accumulated profits or losses of the company that have not been distributed to shareholders as dividends.</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>202345.01</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G60" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H60" s="2" t="inlineStr"/>
+      <c r="I60" s="2" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>balance_sheet.equity.other_comprehensive_income</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>The gains or losses that are not included in net income but are reported directly in equity, such as unrealized gains on investments or foreign currency translation adjustments.</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
+          <t>10987.01</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G61" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H61" s="2" t="inlineStr"/>
+      <c r="I61" s="2" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>balance_sheet.equity.controlling_interest</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>The ownership interest in the company held by the parent entity or majority shareholders, representing the controlling stake in the business.</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>70876.01</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G62" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H62" s="2" t="inlineStr"/>
+      <c r="I62" s="2" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>balance_sheet.equity.non_controlling_interest</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
+        <is>
+          <t>The ownership interest in the company held by minority shareholders, representing the non-controlling stake in the business.</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
+          <t>50321.01</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G63" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H63" s="2" t="inlineStr"/>
+      <c r="I63" s="2" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>balance_sheet.equity.total</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>The sum of share capital, retained earnings, other comprehensive income, controlling interest, and non-controlling interest, representing the total equity of the company.</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>836763.01</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G64" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H64" s="2" t="inlineStr"/>
+      <c r="I64" s="2" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>income_statement</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
+        <is>
+          <t>The income statement detailing the company's revenues, expenses, and profits for the given year.</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="inlineStr"/>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr"/>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G65" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H65" s="2" t="inlineStr"/>
+      <c r="I65" s="2" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
           <t>income_statement.net_revenue</t>
         </is>
       </c>
-      <c r="B59" s="2" t="inlineStr">
+      <c r="B66" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">The total revenue generated by the company from its core business operations, excluding any deductions for discounts, returns, or allowances.
 &gt; **Note**: `domestic_sales` +  `foreign_sales` will not sum to the `net_revenue` due to the exclusion of discounts, returns, and allowances.
 </t>
         </is>
       </c>
-      <c r="C59" s="2" t="inlineStr">
-        <is>
-          <t>1212345</t>
-        </is>
-      </c>
-      <c r="D59" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E59" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F59" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G59" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H59" s="2" t="inlineStr"/>
-      <c r="I59" s="2" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.domestic_sales</t>
-        </is>
-      </c>
-      <c r="B60" s="2" t="inlineStr">
-        <is>
-          <t>The revenue generated by the company from sales of goods or services within its home country.</t>
-        </is>
-      </c>
-      <c r="C60" s="2" t="inlineStr">
-        <is>
-          <t>1123456</t>
-        </is>
-      </c>
-      <c r="D60" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E60" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F60" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G60" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H60" s="2" t="inlineStr"/>
-      <c r="I60" s="2" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.foreign_sales</t>
-        </is>
-      </c>
-      <c r="B61" s="2" t="inlineStr">
-        <is>
-          <t>The revenue generated by the company from sales of goods or services in foreign countries.</t>
-        </is>
-      </c>
-      <c r="C61" s="2" t="inlineStr">
-        <is>
-          <t>88987</t>
-        </is>
-      </c>
-      <c r="D61" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E61" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F61" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G61" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H61" s="2" t="inlineStr"/>
-      <c r="I61" s="2" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.materials_used</t>
-        </is>
-      </c>
-      <c r="B62" s="2" t="inlineStr">
-        <is>
-          <t>The total cost of materials used or traded by the company during the reporting period.</t>
-        </is>
-      </c>
-      <c r="C62" s="2" t="inlineStr">
-        <is>
-          <t>609876</t>
-        </is>
-      </c>
-      <c r="D62" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E62" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F62" s="2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G62" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H62" s="2" t="inlineStr"/>
-      <c r="I62" s="2" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.cost_of_goods_sold</t>
-        </is>
-      </c>
-      <c r="B63" s="2" t="inlineStr">
-        <is>
-          <t>The total cost incurred by the company to produce or purchase the goods sold during the reporting period.</t>
-        </is>
-      </c>
-      <c r="C63" s="2" t="inlineStr">
-        <is>
-          <t>412345</t>
-        </is>
-      </c>
-      <c r="D63" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E63" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F63" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G63" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H63" s="2" t="inlineStr"/>
-      <c r="I63" s="2" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.cost_of_services_sold</t>
-        </is>
-      </c>
-      <c r="B64" s="2" t="inlineStr">
-        <is>
-          <t>The total cost incurred by the company to provide the services sold during the reporting period.</t>
-        </is>
-      </c>
-      <c r="C64" s="2" t="inlineStr">
-        <is>
-          <t>101234</t>
-        </is>
-      </c>
-      <c r="D64" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E64" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F64" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G64" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H64" s="2" t="inlineStr"/>
-      <c r="I64" s="2" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.gross_profit</t>
-        </is>
-      </c>
-      <c r="B65" s="2" t="inlineStr">
-        <is>
-          <t>The difference between net revenue and the total cost of goods and services sold, representing the profit earned from core business operations before deducting operating expenses.</t>
-        </is>
-      </c>
-      <c r="C65" s="2" t="inlineStr">
-        <is>
-          <t>190890</t>
-        </is>
-      </c>
-      <c r="D65" s="2" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="E65" s="2" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F65" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G65" s="2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="H65" s="2" t="inlineStr"/>
-      <c r="I65" s="2" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="2" t="inlineStr">
-        <is>
-          <t>income_statement.gross_loss</t>
-        </is>
-      </c>
-      <c r="B66" s="2" t="inlineStr">
-        <is>
-          <t>The negative difference between net revenue and the total cost of goods and services sold, representing the loss incurred from core business operations before deducting operating expenses.</t>
-        </is>
-      </c>
-      <c r="C66" s="2" t="inlineStr"/>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>1212345.01</t>
+        </is>
+      </c>
       <c r="D66" s="2" t="inlineStr">
         <is>
           <t>number</t>
@@ -29631,17 +29635,17 @@
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>income_statement.operating_expenses</t>
+          <t>income_statement.domestic_sales</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>The total expenses incurred by the company in its normal operating activities, including selling, general, and administrative expenses.</t>
+          <t>The revenue generated by the company from sales of goods or services within its home country.</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>122345</t>
+          <t>1123456.01</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr">
@@ -29670,17 +29674,17 @@
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>income_statement.operating_income</t>
+          <t>income_statement.foreign_sales</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>The profit earned from core business operations after deducting operating expenses, but before considering interest, taxes, and other non-operating items.</t>
+          <t>The revenue generated by the company from sales of goods or services in foreign countries.</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>68545</t>
+          <t>88987.01</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr">
@@ -29709,15 +29713,19 @@
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>income_statement.operating_loss</t>
+          <t>income_statement.materials_used</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>The loss incurred from core business operations after deducting operating expenses, but before considering interest, taxes, and other non-operating items.</t>
-        </is>
-      </c>
-      <c r="C69" s="2" t="inlineStr"/>
+          <t>The total cost of materials used or traded by the company during the reporting period.</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>609876.01</t>
+        </is>
+      </c>
       <c r="D69" s="2" t="inlineStr">
         <is>
           <t>number</t>
@@ -29744,17 +29752,17 @@
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>income_statement.financial_result</t>
+          <t>income_statement.cost_of_goods_sold</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>The net result of financial activities, including interest income, interest expense, and other financial gains or losses.</t>
+          <t>The total cost incurred by the company to produce or purchase the goods sold during the reporting period.</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>15098</t>
+          <t>412345.01</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
@@ -29783,17 +29791,17 @@
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>income_statement.equity_in_earnings_of_affiliates</t>
+          <t>income_statement.cost_of_services_sold</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>The company's share of the profit or loss in its associates, entities over which it has significant influence but not control.</t>
+          <t>The total cost incurred by the company to provide the services sold during the reporting period.</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>5678</t>
+          <t>101234.01</t>
         </is>
       </c>
       <c r="D71" s="2" t="inlineStr">
@@ -29822,17 +29830,17 @@
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>income_statement.income_before_taxes</t>
+          <t>income_statement.gross_profit</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>The profit earned before accounting for income tax expenses.</t>
+          <t>The difference between net revenue and the total cost of goods and services sold, representing the profit earned from core business operations before deducting operating expenses.</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>89321</t>
+          <t>190890.01</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
@@ -29861,12 +29869,12 @@
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>income_statement.loss_before_taxes</t>
+          <t>income_statement.gross_loss</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>The loss incurred before accounting for income tax expenses.</t>
+          <t>The negative difference between net revenue and the total cost of goods and services sold, representing the loss incurred from core business operations before deducting operating expenses.</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr"/>
@@ -29896,17 +29904,17 @@
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>income_statement.income_taxes</t>
+          <t>income_statement.operating_expenses</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>The total amount of income tax expenses incurred during the reporting period.</t>
+          <t>The total expenses incurred by the company in its normal operating activities, including selling, general, and administrative expenses.</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>20123</t>
+          <t>122345.01</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
@@ -29935,17 +29943,17 @@
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>income_statement.income_from_continuing_operations</t>
+          <t>income_statement.operating_income</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>The profit earned from the company's ongoing business operations after deducting operating expenses and taxes.</t>
+          <t>The profit earned from core business operations after deducting operating expenses, but before considering interest, taxes, and other non-operating items.</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>69198</t>
+          <t>68545.01</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
@@ -29974,12 +29982,12 @@
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>income_statement.loss_from_continuing_operations</t>
+          <t>income_statement.operating_loss</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>The loss incurred from the company's ongoing business operations after deducting operating expenses and taxes.</t>
+          <t>The loss incurred from core business operations after deducting operating expenses, but before considering interest, taxes, and other non-operating items.</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr"/>
@@ -30009,17 +30017,17 @@
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>income_statement.discontinued_operations</t>
+          <t>income_statement.financial_result</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>The net result of operations that have been discontinued or sold off during the reporting period.</t>
+          <t>The net result of financial activities, including interest income, interest expense, and other financial gains or losses.</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>15098.01</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr">
@@ -30048,17 +30056,17 @@
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>income_statement.net_income</t>
+          <t>income_statement.income_statement_financial_gains</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>The total profit earned by the company after deducting all expenses, including operating, non-operating, interest, and taxes.</t>
+          <t>The total positive financial income, including interest income, foreign exchange gains, and other gains from financing activities. This value must always be positive.</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>69198</t>
+          <t>85000.01</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
@@ -30087,15 +30095,19 @@
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>income_statement.net_loss</t>
+          <t>income_statement.income_statement_financial_costs</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>The total loss incurred by the company after deducting all expenses, including operating, non-operating, interest, and taxes.</t>
-        </is>
-      </c>
-      <c r="C79" s="2" t="inlineStr"/>
+          <t>The total financial expenses, including interest expenses, foreign exchange losses, and other costs incurred from financing activities. This value must always be negative.</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>-32000.01</t>
+        </is>
+      </c>
       <c r="D79" s="2" t="inlineStr">
         <is>
           <t>number</t>
@@ -30118,6 +30130,345 @@
       </c>
       <c r="H79" s="2" t="inlineStr"/>
       <c r="I79" s="2" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.equity_in_earnings_of_affiliates</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>The company's share of the profit or loss in its associates, entities over which it has significant influence but not control.</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>5678.01</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G80" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H80" s="2" t="inlineStr"/>
+      <c r="I80" s="2" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.income_before_taxes</t>
+        </is>
+      </c>
+      <c r="B81" s="2" t="inlineStr">
+        <is>
+          <t>The profit earned before accounting for income tax expenses.</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
+          <t>89321.01</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F81" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G81" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H81" s="2" t="inlineStr"/>
+      <c r="I81" s="2" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.loss_before_taxes</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>The loss incurred before accounting for income tax expenses.</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr"/>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F82" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G82" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H82" s="2" t="inlineStr"/>
+      <c r="I82" s="2" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.income_taxes</t>
+        </is>
+      </c>
+      <c r="B83" s="2" t="inlineStr">
+        <is>
+          <t>The total amount of income tax expenses incurred during the reporting period.</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="inlineStr">
+        <is>
+          <t>20123.01</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F83" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G83" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H83" s="2" t="inlineStr"/>
+      <c r="I83" s="2" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.income_from_continuing_operations</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>The profit earned from the company's ongoing business operations after deducting operating expenses and taxes.</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>69198.01</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F84" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G84" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H84" s="2" t="inlineStr"/>
+      <c r="I84" s="2" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.loss_from_continuing_operations</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="inlineStr">
+        <is>
+          <t>The loss incurred from the company's ongoing business operations after deducting operating expenses and taxes.</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="inlineStr"/>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F85" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G85" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H85" s="2" t="inlineStr"/>
+      <c r="I85" s="2" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.discontinued_operations</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>The net result of operations that have been discontinued or sold off during the reporting period.</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F86" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G86" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H86" s="2" t="inlineStr"/>
+      <c r="I86" s="2" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.net_income</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="inlineStr">
+        <is>
+          <t>The total profit earned by the company after deducting all expenses, including operating, non-operating, interest, and taxes.</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="inlineStr">
+        <is>
+          <t>69198.01</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F87" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G87" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H87" s="2" t="inlineStr"/>
+      <c r="I87" s="2" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>income_statement.net_loss</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>The total loss incurred by the company after deducting all expenses, including operating, non-operating, interest, and taxes.</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr"/>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G88" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H88" s="2" t="inlineStr"/>
+      <c r="I88" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -30620,7 +30971,7 @@
           <t xml:space="preserve">Indicates whether or not to store credentials (and the duration for which to store the credentials).
 - For recurrent links, this is set to `store` by default (and cannot be changed). 
 - For single links, this is set to `365d` by default.
-Choose either:
+Can be either:
   - `store` to store credentials (until the link is deleted)
   - `nostore` to not store credentials
   -  Any value between `1d` and `365d` to indicate the number of days you want the credentials to be stored.

</xml_diff>

<commit_message>
Sync data dictionaries from public_api_docs (#30)
Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data_dictionaries/en/Belvo_Data_Dictionary_en.xlsx
+++ b/data_dictionaries/en/Belvo_Data_Dictionary_en.xlsx
@@ -11268,13 +11268,15 @@
 We return one of the following values:
   - `REGULAR`
   - `THIRTEENTH`
+  - `VOLUNTARY`
+  - `RETIREMENT`
   - `null`
 </t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>REGULAR</t>
+          <t>VOLUNTARY</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -11295,7 +11297,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>REGULAR, THIRTEENTH, None</t>
+          <t>REGULAR, THIRTEENTH, VOLUNTARY, RETIREMENT, None</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr"/>

</xml_diff>